<commit_message>
Updates to v1.2 : Made two screw terminals DNPs, and changed C2 from .1uf to 1uF to help with preventing resetting of PIC32 when RN does firmware update.
</commit_message>
<xml_diff>
--- a/board_v12/RGB_Station_v12_BOM_Microchip.xlsx
+++ b/board_v12/RGB_Station_v12_BOM_Microchip.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -145,9 +145,6 @@
     <t>IC1</t>
   </si>
   <si>
-    <t>C3</t>
-  </si>
-  <si>
     <t>PRG, RESET</t>
   </si>
   <si>
@@ -283,9 +280,6 @@
     <t>Stackpole</t>
   </si>
   <si>
-    <t>C2, C4, C6, C7, C8, C9, C10, C14</t>
-  </si>
-  <si>
     <t>LED3</t>
   </si>
   <si>
@@ -451,16 +445,22 @@
     <t>629105136821</t>
   </si>
   <si>
-    <t>Bill of Materials For Project RGB Station v1.1</t>
-  </si>
-  <si>
-    <t>RGB Station v1.1 blank PCB</t>
-  </si>
-  <si>
     <t>MCP131T-315E/TT</t>
   </si>
   <si>
     <t>MCP131T-315E/TTCT-ND</t>
+  </si>
+  <si>
+    <t>Bill of Materials For Project RGB Station</t>
+  </si>
+  <si>
+    <t>RGB Station v1.2 blank PCB</t>
+  </si>
+  <si>
+    <t>C2, C3</t>
+  </si>
+  <si>
+    <t>C4, C6, C7, C8, C9, C10, C14</t>
   </si>
 </sst>
 </file>
@@ -1155,9 +1155,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1326,6 +1323,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1680,10 +1680,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1714,14 +1714,14 @@
       <c r="J1" s="34"/>
       <c r="K1" s="34"/>
       <c r="L1" s="34"/>
-      <c r="M1" s="62"/>
+      <c r="M1" s="61"/>
     </row>
     <row r="2" spans="1:13" ht="37.5" customHeight="1" thickBot="1">
       <c r="C2" s="26" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="22"/>
-      <c r="E2" s="77" t="s">
+      <c r="E2" s="76" t="s">
         <v>142</v>
       </c>
       <c r="F2" s="4"/>
@@ -1730,29 +1730,29 @@
       <c r="I2" s="56"/>
       <c r="J2" s="56"/>
       <c r="K2" s="56"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="63"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="62"/>
     </row>
     <row r="3" spans="1:13" ht="23.25" customHeight="1">
       <c r="C3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="74"/>
+      <c r="D3" s="73"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="127"/>
-      <c r="L3" s="124"/>
-      <c r="M3" s="64"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="123"/>
+      <c r="M3" s="63"/>
     </row>
     <row r="4" spans="1:13" ht="17.25" customHeight="1">
       <c r="C4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="75">
+      <c r="D4" s="74">
         <v>1.2</v>
       </c>
       <c r="E4" s="2"/>
@@ -1761,16 +1761,16 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="128"/>
-      <c r="L4" s="125"/>
+      <c r="K4" s="127"/>
+      <c r="L4" s="124"/>
       <c r="M4" s="6"/>
     </row>
     <row r="5" spans="1:13" ht="17.25" customHeight="1">
       <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="76" t="s">
-        <v>56</v>
+      <c r="D5" s="75" t="s">
+        <v>55</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1778,16 +1778,16 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="128"/>
-      <c r="L5" s="125"/>
+      <c r="K5" s="127"/>
+      <c r="L5" s="124"/>
       <c r="M5" s="6"/>
     </row>
     <row r="6" spans="1:13" ht="17.25" customHeight="1">
       <c r="C6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="76" t="s">
-        <v>56</v>
+      <c r="D6" s="75" t="s">
+        <v>55</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -1795,8 +1795,8 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="128"/>
-      <c r="L6" s="125"/>
+      <c r="K6" s="127"/>
+      <c r="L6" s="124"/>
       <c r="M6" s="6"/>
     </row>
     <row r="7" spans="1:13">
@@ -1806,17 +1806,17 @@
       <c r="F7" s="45"/>
       <c r="G7" s="45"/>
       <c r="H7" s="45"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="129"/>
-      <c r="L7" s="126"/>
-      <c r="M7" s="60"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="84"/>
+      <c r="K7" s="128"/>
+      <c r="L7" s="125"/>
+      <c r="M7" s="59"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1">
       <c r="C8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="73"/>
+      <c r="D8" s="72"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1825,13 +1825,13 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="71"/>
+      <c r="M8" s="70"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1">
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="73"/>
+      <c r="D9" s="72"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1840,7 +1840,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="72"/>
+      <c r="M9" s="71"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1">
       <c r="C10" s="1"/>
@@ -1853,43 +1853,43 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-      <c r="M10" s="60"/>
+      <c r="M10" s="59"/>
     </row>
     <row r="11" spans="1:13" s="25" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="77" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="79" t="s">
+      <c r="D11" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="79" t="s">
+      <c r="E11" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="79" t="s">
+      <c r="F11" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="79" t="s">
+      <c r="G11" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="79" t="s">
+      <c r="H11" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="79" t="s">
+      <c r="I11" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="86" t="s">
+      <c r="J11" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="K11" s="79" t="s">
+      <c r="K11" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="L11" s="79" t="s">
+      <c r="L11" s="78" t="s">
         <v>36</v>
       </c>
       <c r="M11" s="55" t="s">
@@ -1900,34 +1900,34 @@
       <c r="A12" s="8">
         <v>4</v>
       </c>
-      <c r="C12" s="114">
-        <v>1</v>
-      </c>
-      <c r="D12" s="87" t="s">
+      <c r="C12" s="113">
+        <v>1</v>
+      </c>
+      <c r="D12" s="86" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="111" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="114" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="92" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="111" t="s">
         <v>62</v>
-      </c>
-      <c r="E12" s="112" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="87" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12" s="115" t="s">
-        <v>65</v>
-      </c>
-      <c r="H12" s="93" t="s">
-        <v>33</v>
-      </c>
-      <c r="I12" s="112" t="s">
-        <v>63</v>
       </c>
       <c r="J12" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K12" s="90">
-        <v>1</v>
-      </c>
-      <c r="L12" s="118">
+      <c r="K12" s="89">
+        <v>1</v>
+      </c>
+      <c r="L12" s="117">
         <v>0.88</v>
       </c>
       <c r="M12" s="54">
@@ -1939,34 +1939,34 @@
       <c r="A13" s="8">
         <v>2</v>
       </c>
-      <c r="C13" s="114">
-        <v>1</v>
-      </c>
-      <c r="D13" s="88" t="s">
+      <c r="C13" s="113">
+        <v>1</v>
+      </c>
+      <c r="D13" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="91" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="92" t="s">
-        <v>50</v>
-      </c>
-      <c r="G13" s="116" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="93" t="s">
+      <c r="E13" s="90" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="91" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="115" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="112" t="s">
-        <v>66</v>
+      <c r="I13" s="111" t="s">
+        <v>65</v>
       </c>
       <c r="J13" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K13" s="90">
-        <v>1</v>
-      </c>
-      <c r="L13" s="118">
+      <c r="K13" s="89">
+        <v>1</v>
+      </c>
+      <c r="L13" s="117">
         <v>0.5</v>
       </c>
       <c r="M13" s="54">
@@ -1978,34 +1978,34 @@
       <c r="A14" s="8">
         <v>1</v>
       </c>
-      <c r="C14" s="114">
-        <v>1</v>
-      </c>
-      <c r="D14" s="89" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="91" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" s="101" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" s="117" t="s">
-        <v>55</v>
-      </c>
-      <c r="H14" s="93" t="s">
+      <c r="C14" s="113">
+        <v>2</v>
+      </c>
+      <c r="D14" s="88" t="s">
+        <v>144</v>
+      </c>
+      <c r="E14" s="90" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="100" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="116" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I14" s="95" t="s">
-        <v>57</v>
+      <c r="I14" s="94" t="s">
+        <v>56</v>
       </c>
       <c r="J14" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K14" s="90">
-        <v>1</v>
-      </c>
-      <c r="L14" s="118">
+      <c r="K14" s="89">
+        <v>1</v>
+      </c>
+      <c r="L14" s="117">
         <v>0.1</v>
       </c>
       <c r="M14" s="54">
@@ -2017,34 +2017,34 @@
       <c r="A15" s="8">
         <v>1</v>
       </c>
-      <c r="C15" s="114">
+      <c r="C15" s="113">
         <v>3</v>
       </c>
-      <c r="D15" s="89" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="120" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="101" t="s">
-        <v>81</v>
-      </c>
-      <c r="G15" s="121" t="s">
-        <v>126</v>
-      </c>
-      <c r="H15" s="93" t="s">
+      <c r="D15" s="88" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="119" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="100" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="120" t="s">
+        <v>124</v>
+      </c>
+      <c r="H15" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I15" s="100" t="s">
-        <v>125</v>
+      <c r="I15" s="99" t="s">
+        <v>123</v>
       </c>
       <c r="J15" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K15" s="90">
+      <c r="K15" s="89">
         <v>3</v>
       </c>
-      <c r="L15" s="118">
+      <c r="L15" s="117">
         <v>0.15</v>
       </c>
       <c r="M15" s="54">
@@ -2056,34 +2056,34 @@
       <c r="A16" s="8">
         <v>1</v>
       </c>
-      <c r="C16" s="114">
-        <v>1</v>
-      </c>
-      <c r="D16" s="89" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="120" t="s">
+      <c r="C16" s="113">
+        <v>1</v>
+      </c>
+      <c r="D16" s="88" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="119" t="s">
+        <v>137</v>
+      </c>
+      <c r="F16" s="112" t="s">
+        <v>138</v>
+      </c>
+      <c r="G16" s="121" t="s">
         <v>139</v>
       </c>
-      <c r="F16" s="113" t="s">
-        <v>140</v>
-      </c>
-      <c r="G16" s="122" t="s">
-        <v>141</v>
-      </c>
-      <c r="H16" s="93" t="s">
+      <c r="H16" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I16" s="100" t="s">
-        <v>138</v>
+      <c r="I16" s="99" t="s">
+        <v>136</v>
       </c>
       <c r="J16" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K16" s="90">
-        <v>1</v>
-      </c>
-      <c r="L16" s="118">
+      <c r="K16" s="89">
+        <v>1</v>
+      </c>
+      <c r="L16" s="117">
         <v>1.21</v>
       </c>
       <c r="M16" s="54">
@@ -2095,34 +2095,34 @@
       <c r="A17" s="8">
         <v>1</v>
       </c>
-      <c r="C17" s="114">
+      <c r="C17" s="113">
         <v>2</v>
       </c>
-      <c r="D17" s="89" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="120" t="s">
+      <c r="D17" s="88" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="119" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="100" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="122" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="101" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="123" t="s">
-        <v>70</v>
-      </c>
-      <c r="H17" s="93" t="s">
+      <c r="H17" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="112" t="s">
-        <v>68</v>
+      <c r="I17" s="111" t="s">
+        <v>67</v>
       </c>
       <c r="J17" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K17" s="90">
+      <c r="K17" s="89">
         <v>2</v>
       </c>
-      <c r="L17" s="118">
+      <c r="L17" s="117">
         <v>0.51</v>
       </c>
       <c r="M17" s="54">
@@ -2134,34 +2134,34 @@
       <c r="A18" s="8">
         <v>1</v>
       </c>
-      <c r="C18" s="114">
-        <v>8</v>
-      </c>
-      <c r="D18" s="89" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" s="120" t="s">
-        <v>82</v>
-      </c>
-      <c r="F18" s="101" t="s">
+      <c r="C18" s="113">
+        <v>7</v>
+      </c>
+      <c r="D18" s="88" t="s">
+        <v>145</v>
+      </c>
+      <c r="E18" s="119" t="s">
         <v>81</v>
       </c>
-      <c r="G18" s="123" t="s">
+      <c r="F18" s="100" t="s">
         <v>80</v>
       </c>
-      <c r="H18" s="93" t="s">
+      <c r="G18" s="122" t="s">
+        <v>79</v>
+      </c>
+      <c r="H18" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I18" s="112" t="s">
-        <v>79</v>
+      <c r="I18" s="111" t="s">
+        <v>78</v>
       </c>
       <c r="J18" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K18" s="90">
+      <c r="K18" s="89">
         <v>8</v>
       </c>
-      <c r="L18" s="118">
+      <c r="L18" s="117">
         <v>0.1</v>
       </c>
       <c r="M18" s="54">
@@ -2173,34 +2173,34 @@
       <c r="A19" s="8">
         <v>2</v>
       </c>
-      <c r="C19" s="114">
-        <v>1</v>
-      </c>
-      <c r="D19" s="89" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="120" t="s">
-        <v>96</v>
-      </c>
-      <c r="F19" s="101" t="s">
+      <c r="C19" s="113">
+        <v>1</v>
+      </c>
+      <c r="D19" s="88" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="119" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="100" t="s">
+        <v>91</v>
+      </c>
+      <c r="G19" s="122" t="s">
         <v>93</v>
       </c>
-      <c r="G19" s="123" t="s">
-        <v>95</v>
-      </c>
-      <c r="H19" s="93" t="s">
+      <c r="H19" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="112" t="s">
-        <v>94</v>
+      <c r="I19" s="111" t="s">
+        <v>92</v>
       </c>
       <c r="J19" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K19" s="90">
-        <v>1</v>
-      </c>
-      <c r="L19" s="118">
+      <c r="K19" s="89">
+        <v>1</v>
+      </c>
+      <c r="L19" s="117">
         <v>0.14000000000000001</v>
       </c>
       <c r="M19" s="54">
@@ -2212,34 +2212,34 @@
       <c r="A20" s="8">
         <v>1</v>
       </c>
-      <c r="C20" s="114">
-        <v>1</v>
-      </c>
-      <c r="D20" s="89" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="120" t="s">
-        <v>99</v>
-      </c>
-      <c r="F20" s="101" t="s">
-        <v>93</v>
-      </c>
-      <c r="G20" s="123" t="s">
-        <v>98</v>
-      </c>
-      <c r="H20" s="93" t="s">
+      <c r="C20" s="113">
+        <v>1</v>
+      </c>
+      <c r="D20" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="119" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="100" t="s">
+        <v>91</v>
+      </c>
+      <c r="G20" s="122" t="s">
+        <v>96</v>
+      </c>
+      <c r="H20" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I20" s="112" t="s">
-        <v>97</v>
+      <c r="I20" s="111" t="s">
+        <v>95</v>
       </c>
       <c r="J20" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K20" s="90">
-        <v>1</v>
-      </c>
-      <c r="L20" s="118">
+      <c r="K20" s="89">
+        <v>1</v>
+      </c>
+      <c r="L20" s="117">
         <v>0.22</v>
       </c>
       <c r="M20" s="54">
@@ -2251,34 +2251,34 @@
       <c r="A21" s="8">
         <v>2</v>
       </c>
-      <c r="C21" s="114">
+      <c r="C21" s="113">
         <v>3</v>
       </c>
-      <c r="D21" s="89" t="s">
-        <v>130</v>
-      </c>
-      <c r="E21" s="120" t="s">
-        <v>137</v>
-      </c>
-      <c r="F21" s="101" t="s">
-        <v>85</v>
-      </c>
-      <c r="G21" s="121" t="s">
-        <v>136</v>
-      </c>
-      <c r="H21" s="93" t="s">
+      <c r="D21" s="88" t="s">
+        <v>128</v>
+      </c>
+      <c r="E21" s="119" t="s">
+        <v>135</v>
+      </c>
+      <c r="F21" s="100" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" s="120" t="s">
+        <v>134</v>
+      </c>
+      <c r="H21" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I21" s="100" t="s">
-        <v>135</v>
+      <c r="I21" s="99" t="s">
+        <v>133</v>
       </c>
       <c r="J21" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K21" s="90">
+      <c r="K21" s="89">
         <v>3</v>
       </c>
-      <c r="L21" s="118">
+      <c r="L21" s="117">
         <v>0.1</v>
       </c>
       <c r="M21" s="54">
@@ -2290,34 +2290,34 @@
       <c r="A22" s="8">
         <v>1</v>
       </c>
-      <c r="C22" s="114">
+      <c r="C22" s="113">
         <v>3</v>
       </c>
-      <c r="D22" s="89" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="91" t="s">
-        <v>48</v>
-      </c>
-      <c r="F22" s="101" t="s">
-        <v>85</v>
-      </c>
-      <c r="G22" s="123" t="s">
+      <c r="D22" s="88" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="90" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="100" t="s">
         <v>84</v>
       </c>
-      <c r="H22" s="93" t="s">
+      <c r="G22" s="122" t="s">
+        <v>83</v>
+      </c>
+      <c r="H22" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I22" s="112" t="s">
-        <v>83</v>
+      <c r="I22" s="111" t="s">
+        <v>82</v>
       </c>
       <c r="J22" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K22" s="90">
+      <c r="K22" s="89">
         <v>3</v>
       </c>
-      <c r="L22" s="118">
+      <c r="L22" s="117">
         <v>0.1</v>
       </c>
       <c r="M22" s="54">
@@ -2329,34 +2329,34 @@
       <c r="A23" s="8">
         <v>4</v>
       </c>
-      <c r="C23" s="114">
-        <v>1</v>
-      </c>
-      <c r="D23" s="89" t="s">
+      <c r="C23" s="113">
+        <v>1</v>
+      </c>
+      <c r="D23" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="91" t="s">
+      <c r="E23" s="90" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="F23" s="101" t="s">
-        <v>50</v>
-      </c>
-      <c r="G23" s="121" t="s">
-        <v>128</v>
-      </c>
-      <c r="H23" s="93" t="s">
+      <c r="G23" s="120" t="s">
+        <v>126</v>
+      </c>
+      <c r="H23" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I23" s="100" t="s">
-        <v>127</v>
+      <c r="I23" s="99" t="s">
+        <v>125</v>
       </c>
       <c r="J23" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K23" s="90">
-        <v>1</v>
-      </c>
-      <c r="L23" s="118">
+      <c r="K23" s="89">
+        <v>1</v>
+      </c>
+      <c r="L23" s="117">
         <v>4.6900000000000004</v>
       </c>
       <c r="M23" s="54">
@@ -2368,34 +2368,34 @@
       <c r="A24" s="8">
         <v>1</v>
       </c>
-      <c r="C24" s="114">
-        <v>1</v>
-      </c>
-      <c r="D24" s="89" t="s">
-        <v>87</v>
-      </c>
-      <c r="E24" s="120" t="s">
-        <v>102</v>
-      </c>
-      <c r="F24" s="101" t="s">
-        <v>93</v>
-      </c>
-      <c r="G24" s="123" t="s">
-        <v>101</v>
-      </c>
-      <c r="H24" s="93" t="s">
+      <c r="C24" s="113">
+        <v>1</v>
+      </c>
+      <c r="D24" s="88" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="119" t="s">
+        <v>100</v>
+      </c>
+      <c r="F24" s="100" t="s">
+        <v>91</v>
+      </c>
+      <c r="G24" s="122" t="s">
+        <v>99</v>
+      </c>
+      <c r="H24" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I24" s="112" t="s">
-        <v>100</v>
+      <c r="I24" s="111" t="s">
+        <v>98</v>
       </c>
       <c r="J24" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K24" s="90">
-        <v>1</v>
-      </c>
-      <c r="L24" s="118">
+      <c r="K24" s="89">
+        <v>1</v>
+      </c>
+      <c r="L24" s="117">
         <v>0.15</v>
       </c>
       <c r="M24" s="54">
@@ -2407,32 +2407,32 @@
       <c r="A25" s="8">
         <v>1</v>
       </c>
-      <c r="C25" s="114">
-        <v>1</v>
-      </c>
-      <c r="D25" s="119"/>
-      <c r="E25" s="91" t="s">
+      <c r="C25" s="113">
+        <v>1</v>
+      </c>
+      <c r="D25" s="118"/>
+      <c r="E25" s="90" t="s">
         <v>143</v>
       </c>
-      <c r="F25" s="101" t="s">
+      <c r="F25" s="100" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" s="115" t="s">
         <v>60</v>
       </c>
-      <c r="G25" s="116" t="s">
-        <v>61</v>
-      </c>
-      <c r="H25" s="102" t="s">
+      <c r="H25" s="101" t="s">
+        <v>59</v>
+      </c>
+      <c r="I25" s="93" t="s">
         <v>60</v>
-      </c>
-      <c r="I25" s="94" t="s">
-        <v>61</v>
       </c>
       <c r="J25" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K25" s="90">
-        <v>1</v>
-      </c>
-      <c r="L25" s="118"/>
+      <c r="K25" s="89">
+        <v>1</v>
+      </c>
+      <c r="L25" s="117"/>
       <c r="M25" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2442,34 +2442,34 @@
       <c r="A26" s="8">
         <v>2</v>
       </c>
-      <c r="C26" s="114">
-        <v>1</v>
-      </c>
-      <c r="D26" s="89" t="s">
+      <c r="C26" s="113">
+        <v>1</v>
+      </c>
+      <c r="D26" s="88" t="s">
+        <v>101</v>
+      </c>
+      <c r="E26" s="119" t="s">
+        <v>105</v>
+      </c>
+      <c r="F26" s="112" t="s">
         <v>103</v>
       </c>
-      <c r="E26" s="120" t="s">
-        <v>107</v>
-      </c>
-      <c r="F26" s="113" t="s">
-        <v>105</v>
-      </c>
-      <c r="G26" s="123" t="s">
-        <v>106</v>
-      </c>
-      <c r="H26" s="93" t="s">
+      <c r="G26" s="122" t="s">
+        <v>104</v>
+      </c>
+      <c r="H26" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I26" s="112" t="s">
-        <v>104</v>
+      <c r="I26" s="111" t="s">
+        <v>102</v>
       </c>
       <c r="J26" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K26" s="90">
-        <v>1</v>
-      </c>
-      <c r="L26" s="118">
+      <c r="K26" s="89">
+        <v>1</v>
+      </c>
+      <c r="L26" s="117">
         <v>0.57999999999999996</v>
       </c>
       <c r="M26" s="54">
@@ -2478,34 +2478,34 @@
       </c>
     </row>
     <row r="27" spans="1:13" s="8" customFormat="1">
-      <c r="C27" s="114">
-        <v>1</v>
-      </c>
-      <c r="D27" s="89" t="s">
+      <c r="C27" s="113">
+        <v>1</v>
+      </c>
+      <c r="D27" s="88" t="s">
+        <v>106</v>
+      </c>
+      <c r="E27" s="119" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27" s="112" t="s">
+        <v>49</v>
+      </c>
+      <c r="G27" s="122" t="s">
         <v>108</v>
       </c>
-      <c r="E27" s="120" t="s">
-        <v>111</v>
-      </c>
-      <c r="F27" s="113" t="s">
-        <v>50</v>
-      </c>
-      <c r="G27" s="123" t="s">
-        <v>110</v>
-      </c>
-      <c r="H27" s="93" t="s">
+      <c r="H27" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I27" s="112" t="s">
-        <v>109</v>
+      <c r="I27" s="111" t="s">
+        <v>107</v>
       </c>
       <c r="J27" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K27" s="90">
-        <v>1</v>
-      </c>
-      <c r="L27" s="118">
+      <c r="K27" s="89">
+        <v>1</v>
+      </c>
+      <c r="L27" s="117">
         <v>7.38</v>
       </c>
       <c r="M27" s="54">
@@ -2514,34 +2514,34 @@
       </c>
     </row>
     <row r="28" spans="1:13" s="8" customFormat="1">
-      <c r="C28" s="114">
-        <v>1</v>
-      </c>
-      <c r="D28" s="89" t="s">
-        <v>112</v>
-      </c>
-      <c r="E28" s="112" t="s">
-        <v>113</v>
-      </c>
-      <c r="F28" s="113" t="s">
-        <v>50</v>
-      </c>
-      <c r="G28" s="103" t="s">
-        <v>144</v>
-      </c>
-      <c r="H28" s="93" t="s">
-        <v>129</v>
-      </c>
-      <c r="I28" s="100" t="s">
-        <v>145</v>
+      <c r="C28" s="113">
+        <v>1</v>
+      </c>
+      <c r="D28" s="88" t="s">
+        <v>110</v>
+      </c>
+      <c r="E28" s="111" t="s">
+        <v>111</v>
+      </c>
+      <c r="F28" s="112" t="s">
+        <v>49</v>
+      </c>
+      <c r="G28" s="102" t="s">
+        <v>140</v>
+      </c>
+      <c r="H28" s="92" t="s">
+        <v>127</v>
+      </c>
+      <c r="I28" s="99" t="s">
+        <v>141</v>
       </c>
       <c r="J28" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K28" s="90">
-        <v>1</v>
-      </c>
-      <c r="L28" s="118">
+      <c r="K28" s="89">
+        <v>1</v>
+      </c>
+      <c r="L28" s="117">
         <v>0.53</v>
       </c>
       <c r="M28" s="54">
@@ -2550,34 +2550,34 @@
       </c>
     </row>
     <row r="29" spans="1:13" s="8" customFormat="1">
-      <c r="C29" s="114">
-        <v>1</v>
-      </c>
-      <c r="D29" s="89" t="s">
+      <c r="C29" s="113">
+        <v>1</v>
+      </c>
+      <c r="D29" s="88" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" s="111" t="s">
+        <v>115</v>
+      </c>
+      <c r="F29" s="112" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" s="114" t="s">
         <v>114</v>
       </c>
-      <c r="E29" s="112" t="s">
-        <v>117</v>
-      </c>
-      <c r="F29" s="113" t="s">
-        <v>53</v>
-      </c>
-      <c r="G29" s="115" t="s">
-        <v>116</v>
-      </c>
-      <c r="H29" s="93" t="s">
+      <c r="H29" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I29" s="112" t="s">
-        <v>115</v>
+      <c r="I29" s="111" t="s">
+        <v>113</v>
       </c>
       <c r="J29" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K29" s="90">
-        <v>1</v>
-      </c>
-      <c r="L29" s="118">
+      <c r="K29" s="89">
+        <v>1</v>
+      </c>
+      <c r="L29" s="117">
         <v>0.31</v>
       </c>
       <c r="M29" s="54">
@@ -2585,107 +2585,37 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="8" customFormat="1">
-      <c r="C30" s="114">
-        <v>1</v>
-      </c>
-      <c r="D30" s="89" t="s">
-        <v>118</v>
-      </c>
-      <c r="E30" s="112" t="s">
-        <v>121</v>
-      </c>
-      <c r="F30" s="113" t="s">
-        <v>120</v>
-      </c>
-      <c r="G30" s="115">
-        <v>1984617</v>
-      </c>
-      <c r="H30" s="93" t="s">
+    <row r="30" spans="1:13" s="8" customFormat="1"/>
+    <row r="31" spans="1:13" s="8" customFormat="1"/>
+    <row r="32" spans="1:13" s="8" customFormat="1">
+      <c r="C32" s="113">
+        <v>2</v>
+      </c>
+      <c r="D32" s="88" t="s">
+        <v>129</v>
+      </c>
+      <c r="E32" s="99" t="s">
+        <v>132</v>
+      </c>
+      <c r="F32" s="100" t="s">
+        <v>84</v>
+      </c>
+      <c r="G32" s="102" t="s">
+        <v>131</v>
+      </c>
+      <c r="H32" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I30" s="112" t="s">
-        <v>119</v>
-      </c>
-      <c r="J30" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="K30" s="90">
-        <v>1</v>
-      </c>
-      <c r="L30" s="118">
-        <v>0.43</v>
-      </c>
-      <c r="M30" s="54">
-        <f t="shared" si="0"/>
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" s="8" customFormat="1">
-      <c r="C31" s="114">
-        <v>1</v>
-      </c>
-      <c r="D31" s="89" t="s">
-        <v>122</v>
-      </c>
-      <c r="E31" s="112" t="s">
-        <v>124</v>
-      </c>
-      <c r="F31" s="113" t="s">
-        <v>120</v>
-      </c>
-      <c r="G31" s="115">
-        <v>1984633</v>
-      </c>
-      <c r="H31" s="93" t="s">
-        <v>33</v>
-      </c>
-      <c r="I31" s="112" t="s">
-        <v>123</v>
-      </c>
-      <c r="J31" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="K31" s="90">
-        <v>1</v>
-      </c>
-      <c r="L31" s="118">
-        <v>0.85</v>
-      </c>
-      <c r="M31" s="54">
-        <f t="shared" si="0"/>
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" s="8" customFormat="1">
-      <c r="C32" s="114">
-        <v>2</v>
-      </c>
-      <c r="D32" s="89" t="s">
-        <v>131</v>
-      </c>
-      <c r="E32" s="100" t="s">
-        <v>134</v>
-      </c>
-      <c r="F32" s="101" t="s">
-        <v>85</v>
-      </c>
-      <c r="G32" s="103" t="s">
-        <v>133</v>
-      </c>
-      <c r="H32" s="93" t="s">
-        <v>33</v>
-      </c>
-      <c r="I32" s="100" t="s">
-        <v>132</v>
+      <c r="I32" s="99" t="s">
+        <v>130</v>
       </c>
       <c r="J32" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K32" s="90">
+      <c r="K32" s="89">
         <v>2</v>
       </c>
-      <c r="L32" s="118">
+      <c r="L32" s="117">
         <v>0.1</v>
       </c>
       <c r="M32" s="54">
@@ -2697,156 +2627,202 @@
       <c r="A33" s="8">
         <v>1</v>
       </c>
-      <c r="C33" s="130" t="s">
-        <v>59</v>
-      </c>
-      <c r="D33" s="131"/>
-      <c r="E33" s="131"/>
-      <c r="F33" s="131"/>
-      <c r="G33" s="131"/>
-      <c r="H33" s="80"/>
-      <c r="I33" s="80"/>
+      <c r="C33" s="129" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" s="130"/>
+      <c r="E33" s="130"/>
+      <c r="F33" s="130"/>
+      <c r="G33" s="130"/>
+      <c r="H33" s="79"/>
+      <c r="I33" s="79"/>
       <c r="J33" s="53"/>
       <c r="K33" s="53"/>
-      <c r="L33" s="118"/>
+      <c r="L33" s="117"/>
       <c r="M33" s="54"/>
     </row>
     <row r="34" spans="1:13" s="8" customFormat="1">
-      <c r="C34" s="58">
+      <c r="C34" s="131">
         <v>0</v>
       </c>
-      <c r="D34" s="87" t="s">
-        <v>88</v>
-      </c>
-      <c r="E34" s="96" t="s">
-        <v>91</v>
-      </c>
-      <c r="F34" s="92"/>
-      <c r="G34" s="96"/>
-      <c r="H34" s="98"/>
-      <c r="I34" s="96"/>
+      <c r="D34" s="86" t="s">
+        <v>86</v>
+      </c>
+      <c r="E34" s="95" t="s">
+        <v>89</v>
+      </c>
+      <c r="F34" s="91"/>
+      <c r="G34" s="95"/>
+      <c r="H34" s="97"/>
+      <c r="I34" s="95"/>
       <c r="J34" s="53"/>
       <c r="K34" s="53"/>
-      <c r="L34" s="118"/>
+      <c r="L34" s="117"/>
       <c r="M34" s="54"/>
     </row>
     <row r="35" spans="1:13" s="8" customFormat="1">
       <c r="A35" s="8">
         <v>1</v>
       </c>
-      <c r="C35" s="58">
+      <c r="C35" s="131">
         <v>0</v>
       </c>
-      <c r="D35" s="87" t="s">
-        <v>89</v>
-      </c>
-      <c r="E35" s="97" t="s">
-        <v>90</v>
-      </c>
-      <c r="F35" s="92"/>
-      <c r="G35" s="97"/>
-      <c r="H35" s="99"/>
-      <c r="I35" s="97"/>
+      <c r="D35" s="86" t="s">
+        <v>87</v>
+      </c>
+      <c r="E35" s="96" t="s">
+        <v>88</v>
+      </c>
+      <c r="F35" s="91"/>
+      <c r="G35" s="96"/>
+      <c r="H35" s="98"/>
+      <c r="I35" s="96"/>
       <c r="J35" s="53"/>
       <c r="K35" s="53"/>
-      <c r="L35" s="118"/>
+      <c r="L35" s="117"/>
       <c r="M35" s="54"/>
     </row>
     <row r="36" spans="1:13" s="8" customFormat="1">
-      <c r="A36" s="8">
-        <v>1</v>
-      </c>
-      <c r="C36" s="58">
+      <c r="C36" s="131">
         <v>0</v>
       </c>
-      <c r="D36" s="87" t="s">
-        <v>58</v>
-      </c>
-      <c r="E36" s="101" t="s">
-        <v>92</v>
-      </c>
-      <c r="F36" s="80"/>
-      <c r="G36" s="80"/>
-      <c r="H36" s="80"/>
-      <c r="I36" s="80"/>
-      <c r="J36" s="53"/>
-      <c r="K36" s="53"/>
-      <c r="L36" s="118"/>
-      <c r="M36" s="54"/>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="C37" s="48"/>
-      <c r="D37" s="49"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="49"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="50"/>
-      <c r="K37" s="50"/>
-      <c r="L37" s="50"/>
-      <c r="M37" s="52">
-        <f>SUM(M12:M36)</f>
+      <c r="D36" s="88" t="s">
+        <v>116</v>
+      </c>
+      <c r="E36" s="111" t="s">
+        <v>119</v>
+      </c>
+      <c r="F36" s="112" t="s">
+        <v>118</v>
+      </c>
+      <c r="G36" s="114">
+        <v>1984617</v>
+      </c>
+      <c r="H36" s="92" t="s">
+        <v>33</v>
+      </c>
+      <c r="I36" s="111" t="s">
+        <v>117</v>
+      </c>
+      <c r="J36" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="K36" s="89">
+        <v>1</v>
+      </c>
+      <c r="L36" s="117">
+        <v>0.43</v>
+      </c>
+      <c r="M36" s="54">
+        <f>K36*L36</f>
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" s="8" customFormat="1">
+      <c r="C37" s="131">
+        <v>0</v>
+      </c>
+      <c r="D37" s="88" t="s">
+        <v>120</v>
+      </c>
+      <c r="E37" s="111" t="s">
+        <v>122</v>
+      </c>
+      <c r="F37" s="112" t="s">
+        <v>118</v>
+      </c>
+      <c r="G37" s="114">
+        <v>1984633</v>
+      </c>
+      <c r="H37" s="92" t="s">
+        <v>33</v>
+      </c>
+      <c r="I37" s="111" t="s">
+        <v>121</v>
+      </c>
+      <c r="J37" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="K37" s="89">
+        <v>1</v>
+      </c>
+      <c r="L37" s="117">
+        <v>0.85</v>
+      </c>
+      <c r="M37" s="54">
+        <f>K37*L37</f>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" s="8" customFormat="1">
+      <c r="A38" s="8">
+        <v>1</v>
+      </c>
+      <c r="C38" s="131">
+        <v>0</v>
+      </c>
+      <c r="D38" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="E38" s="100" t="s">
+        <v>90</v>
+      </c>
+      <c r="F38" s="79"/>
+      <c r="G38" s="79"/>
+      <c r="H38" s="79"/>
+      <c r="I38" s="79"/>
+      <c r="J38" s="53"/>
+      <c r="K38" s="53"/>
+      <c r="L38" s="117"/>
+      <c r="M38" s="54"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="C39" s="48"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="49"/>
+      <c r="H39" s="49"/>
+      <c r="I39" s="50"/>
+      <c r="J39" s="50"/>
+      <c r="K39" s="50"/>
+      <c r="L39" s="50"/>
+      <c r="M39" s="52">
+        <f>SUM(M12:M38)</f>
         <v>21.04</v>
       </c>
     </row>
-    <row r="38" spans="1:13" customFormat="1" ht="13.7" customHeight="1">
-      <c r="C38" s="35" t="s">
+    <row r="40" spans="1:13" customFormat="1" ht="13.7" customHeight="1">
+      <c r="C40" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D38" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="47"/>
-      <c r="I38" s="47"/>
-      <c r="J38" s="47"/>
-      <c r="K38" s="47"/>
-      <c r="L38" s="27"/>
-      <c r="M38" s="41" t="s">
+      <c r="D40" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="E40" s="47"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="47"/>
+      <c r="H40" s="47"/>
+      <c r="I40" s="47"/>
+      <c r="J40" s="47"/>
+      <c r="K40" s="47"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="41" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
-      <c r="C39" s="38"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="40"/>
-      <c r="F39" s="51"/>
-      <c r="G39" s="51"/>
-      <c r="H39" s="51"/>
-      <c r="I39" s="51"/>
-      <c r="J39" s="51"/>
-      <c r="K39" s="51"/>
-      <c r="L39" s="51"/>
-      <c r="M39" s="68"/>
-    </row>
-    <row r="40" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
-      <c r="C40" s="36"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="27"/>
-      <c r="I40" s="27"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="27"/>
-      <c r="L40" s="27"/>
-      <c r="M40" s="69"/>
-    </row>
     <row r="41" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
-      <c r="C41" s="36"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="27"/>
-      <c r="H41" s="27"/>
-      <c r="I41" s="27"/>
-      <c r="J41" s="27"/>
-      <c r="K41" s="27"/>
-      <c r="L41" s="27"/>
-      <c r="M41" s="69"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="51"/>
+      <c r="H41" s="51"/>
+      <c r="I41" s="51"/>
+      <c r="J41" s="51"/>
+      <c r="K41" s="51"/>
+      <c r="L41" s="51"/>
+      <c r="M41" s="67"/>
     </row>
     <row r="42" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
       <c r="C42" s="36"/>
@@ -2859,59 +2835,85 @@
       <c r="J42" s="27"/>
       <c r="K42" s="27"/>
       <c r="L42" s="27"/>
-      <c r="M42" s="69"/>
-    </row>
-    <row r="43" spans="1:13" customFormat="1" ht="9.75" customHeight="1">
-      <c r="C43" s="37"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="29"/>
-      <c r="K43" s="29"/>
-      <c r="L43" s="29"/>
-      <c r="M43" s="70"/>
+      <c r="M42" s="68"/>
+    </row>
+    <row r="43" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
+      <c r="C43" s="36"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="27"/>
+      <c r="M43" s="68"/>
     </row>
     <row r="44" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
-      <c r="C44" s="37"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
-      <c r="K44" s="29"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="67"/>
-    </row>
-    <row r="45" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
-      <c r="C45" s="16"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
-      <c r="M45" s="65"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="27"/>
+      <c r="L44" s="27"/>
+      <c r="M44" s="68"/>
+    </row>
+    <row r="45" spans="1:13" customFormat="1" ht="9.75" customHeight="1">
+      <c r="C45" s="37"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="43"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="29"/>
+      <c r="K45" s="29"/>
+      <c r="L45" s="29"/>
+      <c r="M45" s="69"/>
     </row>
     <row r="46" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
-      <c r="C46" s="19"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
-      <c r="K46" s="21"/>
-      <c r="L46" s="21"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
+      <c r="K46" s="29"/>
+      <c r="L46" s="29"/>
       <c r="M46" s="66"/>
+    </row>
+    <row r="47" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
+      <c r="C47" s="16"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="64"/>
+    </row>
+    <row r="48" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
+      <c r="C48" s="19"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="21"/>
+      <c r="K48" s="21"/>
+      <c r="L48" s="21"/>
+      <c r="M48" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2950,85 +2952,85 @@
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="81"/>
+      <c r="B1" s="80"/>
     </row>
     <row r="2" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="82"/>
+      <c r="B2" s="81"/>
     </row>
     <row r="3" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="83"/>
+      <c r="B3" s="82"/>
     </row>
     <row r="4" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="82"/>
+      <c r="B4" s="81"/>
     </row>
     <row r="5" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="83"/>
+      <c r="B5" s="82"/>
     </row>
     <row r="6" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="82"/>
+      <c r="B6" s="81"/>
     </row>
     <row r="7" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="83"/>
+      <c r="B7" s="82"/>
     </row>
     <row r="8" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="82"/>
+      <c r="B8" s="81"/>
     </row>
     <row r="9" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="83"/>
+      <c r="B9" s="82"/>
     </row>
     <row r="10" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="82"/>
+      <c r="B10" s="81"/>
     </row>
     <row r="11" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A11" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="83"/>
+      <c r="B11" s="82"/>
     </row>
     <row r="12" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A12" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="82"/>
+      <c r="B12" s="81"/>
     </row>
     <row r="13" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1">
       <c r="A13" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="83"/>
+      <c r="B13" s="82"/>
     </row>
     <row r="14" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" thickBot="1">
       <c r="A14" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="84"/>
+      <c r="B14" s="83"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -3053,92 +3055,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6">
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="103" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="103"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2" s="103" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="104"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-    </row>
-    <row r="2" spans="2:6">
-      <c r="B2" s="104" t="s">
+      <c r="C2" s="103"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="107"/>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+    </row>
+    <row r="4" spans="2:6" ht="25.5">
+      <c r="B4" s="104" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-    </row>
-    <row r="3" spans="2:6">
-      <c r="B3" s="105"/>
-      <c r="C3" s="105"/>
-      <c r="D3" s="109"/>
-      <c r="E3" s="109"/>
-      <c r="F3" s="109"/>
-    </row>
-    <row r="4" spans="2:6" ht="25.5">
-      <c r="B4" s="105" t="s">
+      <c r="C4" s="104"/>
+      <c r="D4" s="108"/>
+      <c r="E4" s="108"/>
+      <c r="F4" s="108"/>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="104"/>
+      <c r="C5" s="104"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="108"/>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="103" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="105"/>
-      <c r="D4" s="109"/>
-      <c r="E4" s="109"/>
-      <c r="F4" s="109"/>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="105"/>
-      <c r="C5" s="105"/>
-      <c r="D5" s="109"/>
-      <c r="E5" s="109"/>
-      <c r="F5" s="109"/>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="104" t="s">
+      <c r="C6" s="103"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="104"/>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108" t="s">
+      <c r="F6" s="107" t="s">
         <v>75</v>
       </c>
-      <c r="F6" s="108" t="s">
+    </row>
+    <row r="7" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B7" s="104"/>
+      <c r="C7" s="104"/>
+      <c r="D7" s="108"/>
+      <c r="E7" s="108"/>
+      <c r="F7" s="108"/>
+    </row>
+    <row r="8" spans="2:6" ht="39" thickBot="1">
+      <c r="B8" s="105" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" ht="13.5" thickBot="1">
-      <c r="B7" s="105"/>
-      <c r="C7" s="105"/>
-      <c r="D7" s="109"/>
-      <c r="E7" s="109"/>
-      <c r="F7" s="109"/>
-    </row>
-    <row r="8" spans="2:6" ht="39" thickBot="1">
-      <c r="B8" s="106" t="s">
+      <c r="C8" s="106"/>
+      <c r="D8" s="109"/>
+      <c r="E8" s="109">
+        <v>1</v>
+      </c>
+      <c r="F8" s="110" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="107"/>
-      <c r="D8" s="110"/>
-      <c r="E8" s="110">
-        <v>1</v>
-      </c>
-      <c r="F8" s="111" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" s="105"/>
-      <c r="C9" s="105"/>
-      <c r="D9" s="109"/>
-      <c r="E9" s="109"/>
-      <c r="F9" s="109"/>
+      <c r="B9" s="104"/>
+      <c r="C9" s="104"/>
+      <c r="D9" s="108"/>
+      <c r="E9" s="108"/>
+      <c r="F9" s="108"/>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="105"/>
-      <c r="C10" s="105"/>
-      <c r="D10" s="109"/>
-      <c r="E10" s="109"/>
-      <c r="F10" s="109"/>
+      <c r="B10" s="104"/>
+      <c r="C10" s="104"/>
+      <c r="D10" s="108"/>
+      <c r="E10" s="108"/>
+      <c r="F10" s="108"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated v1.2 board for PCB:NG production - changed DRC rules to minimize violations. Updated .1uF cap and red LED with alternate parts. Updated USB footprint to be exactly correct for Wurth USB connector from BOM
</commit_message>
<xml_diff>
--- a/board_v12/RGB_Station_v12_BOM_Microchip.xlsx
+++ b/board_v12/RGB_Station_v12_BOM_Microchip.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="148">
   <si>
     <t>Approved</t>
   </si>
@@ -259,12 +259,6 @@
     <t>Excel 97-2003</t>
   </si>
   <si>
-    <t>1276-1033-1-ND</t>
-  </si>
-  <si>
-    <t>CL10B104JB8NNNC</t>
-  </si>
-  <si>
     <t>Samsung</t>
   </si>
   <si>
@@ -301,12 +295,6 @@
     <t>Wurth Electronics</t>
   </si>
   <si>
-    <t>732-4978-1-ND</t>
-  </si>
-  <si>
-    <t>150060RS75000</t>
-  </si>
-  <si>
     <t>LED RED CLEAR 0603 SMD</t>
   </si>
   <si>
@@ -461,6 +449,24 @@
   </si>
   <si>
     <t>C4, C6, C7, C8, C9, C10, C14</t>
+  </si>
+  <si>
+    <t>490-5798-1-ND</t>
+  </si>
+  <si>
+    <t>GCJ188R71H104KA12D</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>350-2030-1-ND</t>
+  </si>
+  <si>
+    <t>5988020107F</t>
+  </si>
+  <si>
+    <t>Dialight</t>
   </si>
 </sst>
 </file>
@@ -979,7 +985,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1300,6 +1306,9 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1324,8 +1333,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1682,8 +1691,8 @@
   </sheetPr>
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1722,7 +1731,7 @@
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="76" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1744,8 +1753,8 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="126"/>
-      <c r="L3" s="123"/>
+      <c r="K3" s="127"/>
+      <c r="L3" s="124"/>
       <c r="M3" s="63"/>
     </row>
     <row r="4" spans="1:13" ht="17.25" customHeight="1">
@@ -1761,8 +1770,8 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="127"/>
-      <c r="L4" s="124"/>
+      <c r="K4" s="128"/>
+      <c r="L4" s="125"/>
       <c r="M4" s="6"/>
     </row>
     <row r="5" spans="1:13" ht="17.25" customHeight="1">
@@ -1778,8 +1787,8 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="127"/>
-      <c r="L5" s="124"/>
+      <c r="K5" s="128"/>
+      <c r="L5" s="125"/>
       <c r="M5" s="6"/>
     </row>
     <row r="6" spans="1:13" ht="17.25" customHeight="1">
@@ -1795,8 +1804,8 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="127"/>
-      <c r="L6" s="124"/>
+      <c r="K6" s="128"/>
+      <c r="L6" s="125"/>
       <c r="M6" s="6"/>
     </row>
     <row r="7" spans="1:13">
@@ -1808,8 +1817,8 @@
       <c r="H7" s="45"/>
       <c r="I7" s="58"/>
       <c r="J7" s="84"/>
-      <c r="K7" s="128"/>
-      <c r="L7" s="125"/>
+      <c r="K7" s="129"/>
+      <c r="L7" s="126"/>
       <c r="M7" s="59"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1">
@@ -1982,7 +1991,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="88" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E14" s="90" t="s">
         <v>45</v>
@@ -2027,16 +2036,16 @@
         <v>46</v>
       </c>
       <c r="F15" s="100" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G15" s="120" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H15" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I15" s="99" t="s">
-        <v>123</v>
+      <c r="I15" s="111" t="s">
+        <v>119</v>
       </c>
       <c r="J15" s="53" t="s">
         <v>37</v>
@@ -2063,19 +2072,19 @@
         <v>57</v>
       </c>
       <c r="E16" s="119" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F16" s="112" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G16" s="121" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H16" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I16" s="99" t="s">
-        <v>136</v>
+      <c r="I16" s="111" t="s">
+        <v>132</v>
       </c>
       <c r="J16" s="53" t="s">
         <v>37</v>
@@ -2138,22 +2147,22 @@
         <v>7</v>
       </c>
       <c r="D18" s="88" t="s">
-        <v>145</v>
-      </c>
-      <c r="E18" s="119" t="s">
-        <v>81</v>
+        <v>141</v>
+      </c>
+      <c r="E18" s="111" t="s">
+        <v>79</v>
       </c>
       <c r="F18" s="100" t="s">
-        <v>80</v>
-      </c>
-      <c r="G18" s="122" t="s">
-        <v>79</v>
+        <v>144</v>
+      </c>
+      <c r="G18" s="132" t="s">
+        <v>143</v>
       </c>
       <c r="H18" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I18" s="111" t="s">
-        <v>78</v>
+        <v>142</v>
       </c>
       <c r="J18" s="53" t="s">
         <v>37</v>
@@ -2162,11 +2171,11 @@
         <v>8</v>
       </c>
       <c r="L18" s="117">
-        <v>0.1</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="M18" s="54">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>1.1200000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:13" s="8" customFormat="1">
@@ -2179,20 +2188,20 @@
       <c r="D19" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="119" t="s">
-        <v>94</v>
+      <c r="E19" s="111" t="s">
+        <v>90</v>
       </c>
       <c r="F19" s="100" t="s">
-        <v>91</v>
-      </c>
-      <c r="G19" s="122" t="s">
-        <v>93</v>
+        <v>147</v>
+      </c>
+      <c r="G19" s="132" t="s">
+        <v>146</v>
       </c>
       <c r="H19" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="111" t="s">
-        <v>92</v>
+      <c r="I19" s="132" t="s">
+        <v>145</v>
       </c>
       <c r="J19" s="53" t="s">
         <v>37</v>
@@ -2201,11 +2210,11 @@
         <v>1</v>
       </c>
       <c r="L19" s="117">
-        <v>0.14000000000000001</v>
+        <v>0.51</v>
       </c>
       <c r="M19" s="54">
         <f>K19*L19</f>
-        <v>0.14000000000000001</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="20" spans="1:13" s="8" customFormat="1">
@@ -2219,19 +2228,19 @@
         <v>42</v>
       </c>
       <c r="E20" s="119" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F20" s="100" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G20" s="122" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H20" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I20" s="111" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J20" s="53" t="s">
         <v>37</v>
@@ -2255,22 +2264,22 @@
         <v>3</v>
       </c>
       <c r="D21" s="88" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E21" s="119" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F21" s="100" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G21" s="120" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H21" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I21" s="99" t="s">
-        <v>133</v>
+      <c r="I21" s="111" t="s">
+        <v>129</v>
       </c>
       <c r="J21" s="53" t="s">
         <v>37</v>
@@ -2300,16 +2309,16 @@
         <v>47</v>
       </c>
       <c r="F22" s="100" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G22" s="122" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H22" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I22" s="111" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J22" s="53" t="s">
         <v>37</v>
@@ -2342,13 +2351,13 @@
         <v>49</v>
       </c>
       <c r="G23" s="120" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="H23" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I23" s="99" t="s">
-        <v>125</v>
+      <c r="I23" s="111" t="s">
+        <v>121</v>
       </c>
       <c r="J23" s="53" t="s">
         <v>37</v>
@@ -2372,22 +2381,22 @@
         <v>1</v>
       </c>
       <c r="D24" s="88" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E24" s="119" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F24" s="100" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G24" s="122" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H24" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I24" s="111" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="J24" s="53" t="s">
         <v>37</v>
@@ -2412,7 +2421,7 @@
       </c>
       <c r="D25" s="118"/>
       <c r="E25" s="90" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F25" s="100" t="s">
         <v>59</v>
@@ -2446,22 +2455,22 @@
         <v>1</v>
       </c>
       <c r="D26" s="88" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" s="119" t="s">
         <v>101</v>
       </c>
-      <c r="E26" s="119" t="s">
-        <v>105</v>
-      </c>
       <c r="F26" s="112" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G26" s="122" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H26" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I26" s="111" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J26" s="53" t="s">
         <v>37</v>
@@ -2482,22 +2491,22 @@
         <v>1</v>
       </c>
       <c r="D27" s="88" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E27" s="119" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F27" s="112" t="s">
         <v>49</v>
       </c>
       <c r="G27" s="122" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H27" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I27" s="111" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J27" s="53" t="s">
         <v>37</v>
@@ -2518,22 +2527,22 @@
         <v>1</v>
       </c>
       <c r="D28" s="88" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E28" s="111" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F28" s="112" t="s">
         <v>49</v>
       </c>
-      <c r="G28" s="102" t="s">
-        <v>140</v>
+      <c r="G28" s="132" t="s">
+        <v>136</v>
       </c>
       <c r="H28" s="92" t="s">
-        <v>127</v>
-      </c>
-      <c r="I28" s="99" t="s">
-        <v>141</v>
+        <v>123</v>
+      </c>
+      <c r="I28" s="111" t="s">
+        <v>137</v>
       </c>
       <c r="J28" s="53" t="s">
         <v>37</v>
@@ -2554,22 +2563,22 @@
         <v>1</v>
       </c>
       <c r="D29" s="88" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E29" s="111" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F29" s="112" t="s">
         <v>52</v>
       </c>
       <c r="G29" s="114" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H29" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I29" s="111" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J29" s="53" t="s">
         <v>37</v>
@@ -2592,22 +2601,22 @@
         <v>2</v>
       </c>
       <c r="D32" s="88" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E32" s="99" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F32" s="100" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G32" s="102" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H32" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I32" s="99" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="J32" s="53" t="s">
         <v>37</v>
@@ -2627,13 +2636,13 @@
       <c r="A33" s="8">
         <v>1</v>
       </c>
-      <c r="C33" s="129" t="s">
+      <c r="C33" s="130" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="130"/>
-      <c r="E33" s="130"/>
-      <c r="F33" s="130"/>
-      <c r="G33" s="130"/>
+      <c r="D33" s="131"/>
+      <c r="E33" s="131"/>
+      <c r="F33" s="131"/>
+      <c r="G33" s="131"/>
       <c r="H33" s="79"/>
       <c r="I33" s="79"/>
       <c r="J33" s="53"/>
@@ -2642,14 +2651,14 @@
       <c r="M33" s="54"/>
     </row>
     <row r="34" spans="1:13" s="8" customFormat="1">
-      <c r="C34" s="131">
+      <c r="C34" s="123">
         <v>0</v>
       </c>
       <c r="D34" s="86" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E34" s="95" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F34" s="91"/>
       <c r="G34" s="95"/>
@@ -2664,14 +2673,14 @@
       <c r="A35" s="8">
         <v>1</v>
       </c>
-      <c r="C35" s="131">
+      <c r="C35" s="123">
         <v>0</v>
       </c>
       <c r="D35" s="86" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E35" s="96" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F35" s="91"/>
       <c r="G35" s="96"/>
@@ -2683,17 +2692,17 @@
       <c r="M35" s="54"/>
     </row>
     <row r="36" spans="1:13" s="8" customFormat="1">
-      <c r="C36" s="131">
+      <c r="C36" s="123">
         <v>0</v>
       </c>
       <c r="D36" s="88" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E36" s="111" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F36" s="112" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G36" s="114">
         <v>1984617</v>
@@ -2702,7 +2711,7 @@
         <v>33</v>
       </c>
       <c r="I36" s="111" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="J36" s="53" t="s">
         <v>37</v>
@@ -2719,17 +2728,17 @@
       </c>
     </row>
     <row r="37" spans="1:13" s="8" customFormat="1">
-      <c r="C37" s="131">
+      <c r="C37" s="123">
         <v>0</v>
       </c>
       <c r="D37" s="88" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E37" s="111" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F37" s="112" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G37" s="114">
         <v>1984633</v>
@@ -2738,7 +2747,7 @@
         <v>33</v>
       </c>
       <c r="I37" s="111" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="J37" s="53" t="s">
         <v>37</v>
@@ -2758,14 +2767,14 @@
       <c r="A38" s="8">
         <v>1</v>
       </c>
-      <c r="C38" s="131">
+      <c r="C38" s="123">
         <v>0</v>
       </c>
       <c r="D38" s="86" t="s">
         <v>57</v>
       </c>
       <c r="E38" s="100" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F38" s="79"/>
       <c r="G38" s="79"/>
@@ -2789,7 +2798,7 @@
       <c r="L39" s="50"/>
       <c r="M39" s="52">
         <f>SUM(M12:M38)</f>
-        <v>21.04</v>
+        <v>21.73</v>
       </c>
     </row>
     <row r="40" spans="1:13" customFormat="1" ht="13.7" customHeight="1">

</xml_diff>

<commit_message>
Updated U2 (level shifter) to alternate part that's available (same package, no board change).
</commit_message>
<xml_diff>
--- a/board_v12/RGB_Station_v12_BOM_Microchip.xlsx
+++ b/board_v12/RGB_Station_v12_BOM_Microchip.xlsx
@@ -310,27 +310,15 @@
     <t>732-4966-1-ND</t>
   </si>
   <si>
-    <t>150060BS75000</t>
-  </si>
-  <si>
     <t>LED BLUE CLEAR 0603 SMD</t>
   </si>
   <si>
     <t>U2</t>
   </si>
   <si>
-    <t>1727-4578-1-ND</t>
-  </si>
-  <si>
-    <t>Nexperia USA Inc.</t>
-  </si>
-  <si>
     <t>74LVC2T45DC,125</t>
   </si>
   <si>
-    <t>TXRX TRANSLATING 3ST 8VSSOP</t>
-  </si>
-  <si>
     <t>U6</t>
   </si>
   <si>
@@ -467,6 +455,18 @@
   </si>
   <si>
     <t>Dialight</t>
+  </si>
+  <si>
+    <t>296-17014-1-ND</t>
+  </si>
+  <si>
+    <t>SN74LVC2T45DCUR</t>
+  </si>
+  <si>
+    <t>IC BUS TRANSCVR 2B N-INV US8</t>
+  </si>
+  <si>
+    <t>Texas Instur</t>
   </si>
 </sst>
 </file>
@@ -1309,6 +1309,9 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1332,9 +1335,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1689,10 +1689,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M48"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="76" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1753,8 +1753,8 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="127"/>
-      <c r="L3" s="124"/>
+      <c r="K3" s="128"/>
+      <c r="L3" s="125"/>
       <c r="M3" s="63"/>
     </row>
     <row r="4" spans="1:13" ht="17.25" customHeight="1">
@@ -1770,8 +1770,8 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="128"/>
-      <c r="L4" s="125"/>
+      <c r="K4" s="129"/>
+      <c r="L4" s="126"/>
       <c r="M4" s="6"/>
     </row>
     <row r="5" spans="1:13" ht="17.25" customHeight="1">
@@ -1787,8 +1787,8 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="128"/>
-      <c r="L5" s="125"/>
+      <c r="K5" s="129"/>
+      <c r="L5" s="126"/>
       <c r="M5" s="6"/>
     </row>
     <row r="6" spans="1:13" ht="17.25" customHeight="1">
@@ -1804,8 +1804,8 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="128"/>
-      <c r="L6" s="125"/>
+      <c r="K6" s="129"/>
+      <c r="L6" s="126"/>
       <c r="M6" s="6"/>
     </row>
     <row r="7" spans="1:13">
@@ -1817,8 +1817,8 @@
       <c r="H7" s="45"/>
       <c r="I7" s="58"/>
       <c r="J7" s="84"/>
-      <c r="K7" s="129"/>
-      <c r="L7" s="126"/>
+      <c r="K7" s="130"/>
+      <c r="L7" s="127"/>
       <c r="M7" s="59"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1">
@@ -1940,7 +1940,7 @@
         <v>0.88</v>
       </c>
       <c r="M12" s="54">
-        <f t="shared" ref="M12:M32" si="0">K12*L12</f>
+        <f t="shared" ref="M12:M30" si="0">K12*L12</f>
         <v>0.88</v>
       </c>
     </row>
@@ -1991,7 +1991,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="88" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E14" s="90" t="s">
         <v>45</v>
@@ -2039,13 +2039,13 @@
         <v>78</v>
       </c>
       <c r="G15" s="120" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H15" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I15" s="111" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J15" s="53" t="s">
         <v>37</v>
@@ -2072,19 +2072,19 @@
         <v>57</v>
       </c>
       <c r="E16" s="119" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F16" s="112" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G16" s="121" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="H16" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I16" s="111" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J16" s="53" t="s">
         <v>37</v>
@@ -2147,22 +2147,22 @@
         <v>7</v>
       </c>
       <c r="D18" s="88" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E18" s="111" t="s">
         <v>79</v>
       </c>
       <c r="F18" s="100" t="s">
-        <v>144</v>
-      </c>
-      <c r="G18" s="132" t="s">
-        <v>143</v>
+        <v>140</v>
+      </c>
+      <c r="G18" s="124" t="s">
+        <v>139</v>
       </c>
       <c r="H18" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I18" s="111" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="J18" s="53" t="s">
         <v>37</v>
@@ -2192,16 +2192,16 @@
         <v>90</v>
       </c>
       <c r="F19" s="100" t="s">
-        <v>147</v>
-      </c>
-      <c r="G19" s="132" t="s">
-        <v>146</v>
+        <v>143</v>
+      </c>
+      <c r="G19" s="124" t="s">
+        <v>142</v>
       </c>
       <c r="H19" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="132" t="s">
-        <v>145</v>
+      <c r="I19" s="124" t="s">
+        <v>141</v>
       </c>
       <c r="J19" s="53" t="s">
         <v>37</v>
@@ -2264,22 +2264,22 @@
         <v>3</v>
       </c>
       <c r="D21" s="88" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E21" s="119" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F21" s="100" t="s">
         <v>82</v>
       </c>
       <c r="G21" s="120" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H21" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I21" s="111" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="J21" s="53" t="s">
         <v>37</v>
@@ -2351,13 +2351,13 @@
         <v>49</v>
       </c>
       <c r="G23" s="120" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H23" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I23" s="111" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="J23" s="53" t="s">
         <v>37</v>
@@ -2384,13 +2384,13 @@
         <v>83</v>
       </c>
       <c r="E24" s="119" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F24" s="100" t="s">
         <v>89</v>
       </c>
-      <c r="G24" s="122" t="s">
-        <v>95</v>
+      <c r="G24" s="102" t="s">
+        <v>145</v>
       </c>
       <c r="H24" s="92" t="s">
         <v>33</v>
@@ -2421,7 +2421,7 @@
       </c>
       <c r="D25" s="118"/>
       <c r="E25" s="90" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F25" s="100" t="s">
         <v>59</v>
@@ -2455,22 +2455,22 @@
         <v>1</v>
       </c>
       <c r="D26" s="88" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" s="99" t="s">
+        <v>146</v>
+      </c>
+      <c r="F26" s="112" t="s">
+        <v>147</v>
+      </c>
+      <c r="G26" s="122" t="s">
         <v>97</v>
-      </c>
-      <c r="E26" s="119" t="s">
-        <v>101</v>
-      </c>
-      <c r="F26" s="112" t="s">
-        <v>99</v>
-      </c>
-      <c r="G26" s="122" t="s">
-        <v>100</v>
       </c>
       <c r="H26" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I26" s="111" t="s">
-        <v>98</v>
+      <c r="I26" s="102" t="s">
+        <v>144</v>
       </c>
       <c r="J26" s="53" t="s">
         <v>37</v>
@@ -2479,11 +2479,11 @@
         <v>1</v>
       </c>
       <c r="L26" s="117">
-        <v>0.57999999999999996</v>
+        <v>0.61</v>
       </c>
       <c r="M26" s="54">
         <f t="shared" si="0"/>
-        <v>0.57999999999999996</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="27" spans="1:13" s="8" customFormat="1">
@@ -2491,22 +2491,22 @@
         <v>1</v>
       </c>
       <c r="D27" s="88" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E27" s="119" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F27" s="112" t="s">
         <v>49</v>
       </c>
       <c r="G27" s="122" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H27" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I27" s="111" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J27" s="53" t="s">
         <v>37</v>
@@ -2527,22 +2527,22 @@
         <v>1</v>
       </c>
       <c r="D28" s="88" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E28" s="111" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F28" s="112" t="s">
         <v>49</v>
       </c>
-      <c r="G28" s="132" t="s">
-        <v>136</v>
+      <c r="G28" s="124" t="s">
+        <v>132</v>
       </c>
       <c r="H28" s="92" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I28" s="111" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J28" s="53" t="s">
         <v>37</v>
@@ -2563,22 +2563,22 @@
         <v>1</v>
       </c>
       <c r="D29" s="88" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E29" s="111" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F29" s="112" t="s">
         <v>52</v>
       </c>
       <c r="G29" s="114" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H29" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I29" s="111" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="J29" s="53" t="s">
         <v>37</v>
@@ -2594,57 +2594,96 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="8" customFormat="1"/>
-    <row r="31" spans="1:13" s="8" customFormat="1"/>
-    <row r="32" spans="1:13" s="8" customFormat="1">
-      <c r="C32" s="113">
+    <row r="30" spans="1:13" s="8" customFormat="1">
+      <c r="C30" s="113">
         <v>2</v>
       </c>
-      <c r="D32" s="88" t="s">
-        <v>125</v>
-      </c>
-      <c r="E32" s="99" t="s">
-        <v>128</v>
-      </c>
-      <c r="F32" s="100" t="s">
+      <c r="D30" s="88" t="s">
+        <v>121</v>
+      </c>
+      <c r="E30" s="99" t="s">
+        <v>124</v>
+      </c>
+      <c r="F30" s="100" t="s">
         <v>82</v>
       </c>
-      <c r="G32" s="102" t="s">
-        <v>127</v>
-      </c>
-      <c r="H32" s="92" t="s">
+      <c r="G30" s="102" t="s">
+        <v>123</v>
+      </c>
+      <c r="H30" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="I32" s="99" t="s">
-        <v>126</v>
-      </c>
-      <c r="J32" s="53" t="s">
+      <c r="I30" s="99" t="s">
+        <v>122</v>
+      </c>
+      <c r="J30" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K32" s="89">
+      <c r="K30" s="89">
         <v>2</v>
       </c>
-      <c r="L32" s="117">
+      <c r="L30" s="117">
         <v>0.1</v>
       </c>
-      <c r="M32" s="54">
+      <c r="M30" s="54">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
+    <row r="31" spans="1:13" s="8" customFormat="1">
+      <c r="A31" s="8">
+        <v>1</v>
+      </c>
+      <c r="C31" s="131" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="132"/>
+      <c r="E31" s="132"/>
+      <c r="F31" s="132"/>
+      <c r="G31" s="132"/>
+      <c r="H31" s="79"/>
+      <c r="I31" s="79"/>
+      <c r="J31" s="53"/>
+      <c r="K31" s="53"/>
+      <c r="L31" s="117"/>
+      <c r="M31" s="54"/>
+    </row>
+    <row r="32" spans="1:13" s="8" customFormat="1">
+      <c r="C32" s="123">
+        <v>0</v>
+      </c>
+      <c r="D32" s="86" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" s="95" t="s">
+        <v>87</v>
+      </c>
+      <c r="F32" s="91"/>
+      <c r="G32" s="95"/>
+      <c r="H32" s="97"/>
+      <c r="I32" s="95"/>
+      <c r="J32" s="53"/>
+      <c r="K32" s="53"/>
+      <c r="L32" s="117"/>
+      <c r="M32" s="54"/>
+    </row>
     <row r="33" spans="1:13" s="8" customFormat="1">
       <c r="A33" s="8">
         <v>1</v>
       </c>
-      <c r="C33" s="130" t="s">
-        <v>58</v>
-      </c>
-      <c r="D33" s="131"/>
-      <c r="E33" s="131"/>
-      <c r="F33" s="131"/>
-      <c r="G33" s="131"/>
-      <c r="H33" s="79"/>
-      <c r="I33" s="79"/>
+      <c r="C33" s="123">
+        <v>0</v>
+      </c>
+      <c r="D33" s="86" t="s">
+        <v>85</v>
+      </c>
+      <c r="E33" s="96" t="s">
+        <v>86</v>
+      </c>
+      <c r="F33" s="91"/>
+      <c r="G33" s="96"/>
+      <c r="H33" s="98"/>
+      <c r="I33" s="96"/>
       <c r="J33" s="53"/>
       <c r="K33" s="53"/>
       <c r="L33" s="117"/>
@@ -2654,184 +2693,169 @@
       <c r="C34" s="123">
         <v>0</v>
       </c>
-      <c r="D34" s="86" t="s">
-        <v>84</v>
-      </c>
-      <c r="E34" s="95" t="s">
-        <v>87</v>
-      </c>
-      <c r="F34" s="91"/>
-      <c r="G34" s="95"/>
-      <c r="H34" s="97"/>
-      <c r="I34" s="95"/>
-      <c r="J34" s="53"/>
-      <c r="K34" s="53"/>
-      <c r="L34" s="117"/>
-      <c r="M34" s="54"/>
+      <c r="D34" s="88" t="s">
+        <v>108</v>
+      </c>
+      <c r="E34" s="111" t="s">
+        <v>111</v>
+      </c>
+      <c r="F34" s="112" t="s">
+        <v>110</v>
+      </c>
+      <c r="G34" s="114">
+        <v>1984617</v>
+      </c>
+      <c r="H34" s="92" t="s">
+        <v>33</v>
+      </c>
+      <c r="I34" s="111" t="s">
+        <v>109</v>
+      </c>
+      <c r="J34" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="K34" s="89">
+        <v>1</v>
+      </c>
+      <c r="L34" s="117">
+        <v>0.43</v>
+      </c>
+      <c r="M34" s="54">
+        <f>K34*L34</f>
+        <v>0.43</v>
+      </c>
     </row>
     <row r="35" spans="1:13" s="8" customFormat="1">
-      <c r="A35" s="8">
-        <v>1</v>
-      </c>
       <c r="C35" s="123">
         <v>0</v>
       </c>
-      <c r="D35" s="86" t="s">
-        <v>85</v>
-      </c>
-      <c r="E35" s="96" t="s">
-        <v>86</v>
-      </c>
-      <c r="F35" s="91"/>
-      <c r="G35" s="96"/>
-      <c r="H35" s="98"/>
-      <c r="I35" s="96"/>
-      <c r="J35" s="53"/>
-      <c r="K35" s="53"/>
-      <c r="L35" s="117"/>
-      <c r="M35" s="54"/>
+      <c r="D35" s="88" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35" s="111" t="s">
+        <v>114</v>
+      </c>
+      <c r="F35" s="112" t="s">
+        <v>110</v>
+      </c>
+      <c r="G35" s="114">
+        <v>1984633</v>
+      </c>
+      <c r="H35" s="92" t="s">
+        <v>33</v>
+      </c>
+      <c r="I35" s="111" t="s">
+        <v>113</v>
+      </c>
+      <c r="J35" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="K35" s="89">
+        <v>1</v>
+      </c>
+      <c r="L35" s="117">
+        <v>0.85</v>
+      </c>
+      <c r="M35" s="54">
+        <f>K35*L35</f>
+        <v>0.85</v>
+      </c>
     </row>
     <row r="36" spans="1:13" s="8" customFormat="1">
+      <c r="A36" s="8">
+        <v>1</v>
+      </c>
       <c r="C36" s="123">
         <v>0</v>
       </c>
-      <c r="D36" s="88" t="s">
-        <v>112</v>
-      </c>
-      <c r="E36" s="111" t="s">
-        <v>115</v>
-      </c>
-      <c r="F36" s="112" t="s">
-        <v>114</v>
-      </c>
-      <c r="G36" s="114">
-        <v>1984617</v>
-      </c>
-      <c r="H36" s="92" t="s">
-        <v>33</v>
-      </c>
-      <c r="I36" s="111" t="s">
-        <v>113</v>
-      </c>
-      <c r="J36" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="K36" s="89">
-        <v>1</v>
-      </c>
-      <c r="L36" s="117">
-        <v>0.43</v>
-      </c>
-      <c r="M36" s="54">
-        <f>K36*L36</f>
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" s="8" customFormat="1">
-      <c r="C37" s="123">
+      <c r="D36" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="100" t="s">
+        <v>88</v>
+      </c>
+      <c r="F36" s="79"/>
+      <c r="G36" s="79"/>
+      <c r="H36" s="79"/>
+      <c r="I36" s="79"/>
+      <c r="J36" s="53"/>
+      <c r="K36" s="53"/>
+      <c r="L36" s="117"/>
+      <c r="M36" s="54"/>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="C37" s="48"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="50"/>
+      <c r="K37" s="50"/>
+      <c r="L37" s="50"/>
+      <c r="M37" s="52">
+        <f>SUM(M12:M36)</f>
+        <v>21.76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" customFormat="1" ht="13.7" customHeight="1">
+      <c r="C38" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D37" s="88" t="s">
-        <v>116</v>
-      </c>
-      <c r="E37" s="111" t="s">
-        <v>118</v>
-      </c>
-      <c r="F37" s="112" t="s">
-        <v>114</v>
-      </c>
-      <c r="G37" s="114">
-        <v>1984633</v>
-      </c>
-      <c r="H37" s="92" t="s">
-        <v>33</v>
-      </c>
-      <c r="I37" s="111" t="s">
-        <v>117</v>
-      </c>
-      <c r="J37" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="K37" s="89">
-        <v>1</v>
-      </c>
-      <c r="L37" s="117">
-        <v>0.85</v>
-      </c>
-      <c r="M37" s="54">
-        <f>K37*L37</f>
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" s="8" customFormat="1">
-      <c r="A38" s="8">
-        <v>1</v>
-      </c>
-      <c r="C38" s="123">
-        <v>0</v>
-      </c>
-      <c r="D38" s="86" t="s">
-        <v>57</v>
-      </c>
-      <c r="E38" s="100" t="s">
-        <v>88</v>
-      </c>
-      <c r="F38" s="79"/>
-      <c r="G38" s="79"/>
-      <c r="H38" s="79"/>
-      <c r="I38" s="79"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="53"/>
-      <c r="L38" s="117"/>
-      <c r="M38" s="54"/>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="C39" s="48"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="49"/>
-      <c r="H39" s="49"/>
-      <c r="I39" s="50"/>
-      <c r="J39" s="50"/>
-      <c r="K39" s="50"/>
-      <c r="L39" s="50"/>
-      <c r="M39" s="52">
-        <f>SUM(M12:M38)</f>
-        <v>21.73</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" customFormat="1" ht="13.7" customHeight="1">
-      <c r="C40" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="D40" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="47"/>
-      <c r="H40" s="47"/>
-      <c r="I40" s="47"/>
-      <c r="J40" s="47"/>
-      <c r="K40" s="47"/>
+      <c r="D38" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="47"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="47"/>
+      <c r="J38" s="47"/>
+      <c r="K38" s="47"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
+      <c r="C39" s="38"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="51"/>
+      <c r="L39" s="51"/>
+      <c r="M39" s="67"/>
+    </row>
+    <row r="40" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
+      <c r="C40" s="36"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
       <c r="L40" s="27"/>
-      <c r="M40" s="41" t="s">
-        <v>4</v>
-      </c>
+      <c r="M40" s="68"/>
     </row>
     <row r="41" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
-      <c r="C41" s="38"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="40"/>
-      <c r="F41" s="51"/>
-      <c r="G41" s="51"/>
-      <c r="H41" s="51"/>
-      <c r="I41" s="51"/>
-      <c r="J41" s="51"/>
-      <c r="K41" s="51"/>
-      <c r="L41" s="51"/>
-      <c r="M41" s="67"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="27"/>
+      <c r="L41" s="27"/>
+      <c r="M41" s="68"/>
     </row>
     <row r="42" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
       <c r="C42" s="36"/>
@@ -2846,89 +2870,63 @@
       <c r="L42" s="27"/>
       <c r="M42" s="68"/>
     </row>
-    <row r="43" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
-      <c r="C43" s="36"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="27"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
-      <c r="K43" s="27"/>
-      <c r="L43" s="27"/>
-      <c r="M43" s="68"/>
+    <row r="43" spans="1:13" customFormat="1" ht="9.75" customHeight="1">
+      <c r="C43" s="37"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
+      <c r="L43" s="29"/>
+      <c r="M43" s="69"/>
     </row>
     <row r="44" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
-      <c r="C44" s="36"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="27"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
-      <c r="K44" s="27"/>
-      <c r="L44" s="27"/>
-      <c r="M44" s="68"/>
-    </row>
-    <row r="45" spans="1:13" customFormat="1" ht="9.75" customHeight="1">
-      <c r="C45" s="37"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="29"/>
-      <c r="J45" s="29"/>
-      <c r="K45" s="29"/>
-      <c r="L45" s="29"/>
-      <c r="M45" s="69"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="29"/>
+      <c r="M44" s="66"/>
+    </row>
+    <row r="45" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
+      <c r="C45" s="16"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="64"/>
     </row>
     <row r="46" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
-      <c r="C46" s="37"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="29"/>
-      <c r="H46" s="29"/>
-      <c r="I46" s="29"/>
-      <c r="J46" s="29"/>
-      <c r="K46" s="29"/>
-      <c r="L46" s="29"/>
-      <c r="M46" s="66"/>
-    </row>
-    <row r="47" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
-      <c r="C47" s="16"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
-      <c r="K47" s="18"/>
-      <c r="L47" s="18"/>
-      <c r="M47" s="64"/>
-    </row>
-    <row r="48" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
-      <c r="C48" s="19"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
-      <c r="I48" s="21"/>
-      <c r="J48" s="21"/>
-      <c r="K48" s="21"/>
-      <c r="L48" s="21"/>
-      <c r="M48" s="65"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="L3:L7"/>
     <mergeCell ref="K3:K7"/>
-    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C31:G31"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Updated refdes for switches to SW1 and SW2.
</commit_message>
<xml_diff>
--- a/board_v12/RGB_Station_v12_BOM_Microchip.xlsx
+++ b/board_v12/RGB_Station_v12_BOM_Microchip.xlsx
@@ -145,9 +145,6 @@
     <t>IC1</t>
   </si>
   <si>
-    <t>PRG, RESET</t>
-  </si>
-  <si>
     <t>LED1</t>
   </si>
   <si>
@@ -467,6 +464,9 @@
   </si>
   <si>
     <t>Texas Instur</t>
+  </si>
+  <si>
+    <t>SW1, SW2</t>
   </si>
 </sst>
 </file>
@@ -1692,7 +1692,7 @@
   <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="76" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1779,7 +1779,7 @@
         <v>20</v>
       </c>
       <c r="D5" s="75" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1796,7 +1796,7 @@
         <v>21</v>
       </c>
       <c r="D6" s="75" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -1913,22 +1913,22 @@
         <v>1</v>
       </c>
       <c r="D12" s="86" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E12" s="111" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="86" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="114" t="s">
         <v>63</v>
-      </c>
-      <c r="F12" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="114" t="s">
-        <v>64</v>
       </c>
       <c r="H12" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I12" s="111" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J12" s="53" t="s">
         <v>37</v>
@@ -1955,19 +1955,19 @@
         <v>39</v>
       </c>
       <c r="E13" s="90" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F13" s="91" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G13" s="115" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H13" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I13" s="111" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J13" s="53" t="s">
         <v>37</v>
@@ -1991,22 +1991,22 @@
         <v>2</v>
       </c>
       <c r="D14" s="88" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E14" s="90" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F14" s="100" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G14" s="116" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H14" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I14" s="94" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J14" s="53" t="s">
         <v>37</v>
@@ -2030,22 +2030,22 @@
         <v>3</v>
       </c>
       <c r="D15" s="88" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E15" s="119" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F15" s="100" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G15" s="120" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H15" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I15" s="111" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J15" s="53" t="s">
         <v>37</v>
@@ -2069,22 +2069,22 @@
         <v>1</v>
       </c>
       <c r="D16" s="88" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" s="119" t="s">
+        <v>128</v>
+      </c>
+      <c r="F16" s="112" t="s">
         <v>129</v>
       </c>
-      <c r="F16" s="112" t="s">
+      <c r="G16" s="121" t="s">
         <v>130</v>
-      </c>
-      <c r="G16" s="121" t="s">
-        <v>131</v>
       </c>
       <c r="H16" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I16" s="111" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J16" s="53" t="s">
         <v>37</v>
@@ -2108,22 +2108,22 @@
         <v>2</v>
       </c>
       <c r="D17" s="88" t="s">
-        <v>40</v>
+        <v>147</v>
       </c>
       <c r="E17" s="119" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="100" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="122" t="s">
         <v>68</v>
-      </c>
-      <c r="F17" s="100" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" s="122" t="s">
-        <v>69</v>
       </c>
       <c r="H17" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I17" s="111" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J17" s="53" t="s">
         <v>37</v>
@@ -2147,22 +2147,22 @@
         <v>7</v>
       </c>
       <c r="D18" s="88" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E18" s="111" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F18" s="100" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G18" s="124" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H18" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I18" s="111" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J18" s="53" t="s">
         <v>37</v>
@@ -2186,22 +2186,22 @@
         <v>1</v>
       </c>
       <c r="D19" s="88" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19" s="111" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F19" s="100" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G19" s="124" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H19" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I19" s="124" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J19" s="53" t="s">
         <v>37</v>
@@ -2225,22 +2225,22 @@
         <v>1</v>
       </c>
       <c r="D20" s="88" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" s="119" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F20" s="100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G20" s="122" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H20" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I20" s="111" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J20" s="53" t="s">
         <v>37</v>
@@ -2264,22 +2264,22 @@
         <v>3</v>
       </c>
       <c r="D21" s="88" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E21" s="119" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F21" s="100" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G21" s="120" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H21" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I21" s="111" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J21" s="53" t="s">
         <v>37</v>
@@ -2303,22 +2303,22 @@
         <v>3</v>
       </c>
       <c r="D22" s="88" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E22" s="90" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F22" s="100" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G22" s="122" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H22" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I22" s="111" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J22" s="53" t="s">
         <v>37</v>
@@ -2345,19 +2345,19 @@
         <v>28</v>
       </c>
       <c r="E23" s="90" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="100" t="s">
         <v>48</v>
       </c>
-      <c r="F23" s="100" t="s">
-        <v>49</v>
-      </c>
       <c r="G23" s="120" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H23" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I23" s="111" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J23" s="53" t="s">
         <v>37</v>
@@ -2381,22 +2381,22 @@
         <v>1</v>
       </c>
       <c r="D24" s="88" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E24" s="119" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F24" s="100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G24" s="102" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H24" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I24" s="111" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J24" s="53" t="s">
         <v>37</v>
@@ -2421,19 +2421,19 @@
       </c>
       <c r="D25" s="118"/>
       <c r="E25" s="90" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F25" s="100" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="115" t="s">
         <v>59</v>
       </c>
-      <c r="G25" s="115" t="s">
-        <v>60</v>
-      </c>
       <c r="H25" s="101" t="s">
+        <v>58</v>
+      </c>
+      <c r="I25" s="93" t="s">
         <v>59</v>
-      </c>
-      <c r="I25" s="93" t="s">
-        <v>60</v>
       </c>
       <c r="J25" s="53" t="s">
         <v>37</v>
@@ -2455,22 +2455,22 @@
         <v>1</v>
       </c>
       <c r="D26" s="88" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="99" t="s">
+        <v>145</v>
+      </c>
+      <c r="F26" s="112" t="s">
+        <v>146</v>
+      </c>
+      <c r="G26" s="122" t="s">
         <v>96</v>
-      </c>
-      <c r="E26" s="99" t="s">
-        <v>146</v>
-      </c>
-      <c r="F26" s="112" t="s">
-        <v>147</v>
-      </c>
-      <c r="G26" s="122" t="s">
-        <v>97</v>
       </c>
       <c r="H26" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I26" s="102" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J26" s="53" t="s">
         <v>37</v>
@@ -2491,22 +2491,22 @@
         <v>1</v>
       </c>
       <c r="D27" s="88" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E27" s="119" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F27" s="112" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G27" s="122" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H27" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I27" s="111" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J27" s="53" t="s">
         <v>37</v>
@@ -2527,22 +2527,22 @@
         <v>1</v>
       </c>
       <c r="D28" s="88" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" s="111" t="s">
         <v>102</v>
       </c>
-      <c r="E28" s="111" t="s">
-        <v>103</v>
-      </c>
       <c r="F28" s="112" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G28" s="124" t="s">
+        <v>131</v>
+      </c>
+      <c r="H28" s="92" t="s">
+        <v>118</v>
+      </c>
+      <c r="I28" s="111" t="s">
         <v>132</v>
-      </c>
-      <c r="H28" s="92" t="s">
-        <v>119</v>
-      </c>
-      <c r="I28" s="111" t="s">
-        <v>133</v>
       </c>
       <c r="J28" s="53" t="s">
         <v>37</v>
@@ -2563,22 +2563,22 @@
         <v>1</v>
       </c>
       <c r="D29" s="88" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E29" s="111" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F29" s="112" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G29" s="114" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H29" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I29" s="111" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J29" s="53" t="s">
         <v>37</v>
@@ -2599,22 +2599,22 @@
         <v>2</v>
       </c>
       <c r="D30" s="88" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E30" s="99" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F30" s="100" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G30" s="102" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H30" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I30" s="99" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J30" s="53" t="s">
         <v>37</v>
@@ -2635,7 +2635,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="131" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D31" s="132"/>
       <c r="E31" s="132"/>
@@ -2653,10 +2653,10 @@
         <v>0</v>
       </c>
       <c r="D32" s="86" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E32" s="95" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F32" s="91"/>
       <c r="G32" s="95"/>
@@ -2675,10 +2675,10 @@
         <v>0</v>
       </c>
       <c r="D33" s="86" t="s">
+        <v>84</v>
+      </c>
+      <c r="E33" s="96" t="s">
         <v>85</v>
-      </c>
-      <c r="E33" s="96" t="s">
-        <v>86</v>
       </c>
       <c r="F33" s="91"/>
       <c r="G33" s="96"/>
@@ -2694,13 +2694,13 @@
         <v>0</v>
       </c>
       <c r="D34" s="88" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E34" s="111" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F34" s="112" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G34" s="114">
         <v>1984617</v>
@@ -2709,7 +2709,7 @@
         <v>33</v>
       </c>
       <c r="I34" s="111" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J34" s="53" t="s">
         <v>37</v>
@@ -2730,13 +2730,13 @@
         <v>0</v>
       </c>
       <c r="D35" s="88" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E35" s="111" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F35" s="112" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G35" s="114">
         <v>1984633</v>
@@ -2745,7 +2745,7 @@
         <v>33</v>
       </c>
       <c r="I35" s="111" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J35" s="53" t="s">
         <v>37</v>
@@ -2769,10 +2769,10 @@
         <v>0</v>
       </c>
       <c r="D36" s="86" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E36" s="100" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F36" s="79"/>
       <c r="G36" s="79"/>
@@ -3063,7 +3063,7 @@
   <sheetData>
     <row r="1" spans="2:6">
       <c r="B1" s="103" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" s="103"/>
       <c r="D1" s="107"/>
@@ -3072,7 +3072,7 @@
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="103" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" s="103"/>
       <c r="D2" s="107"/>
@@ -3088,7 +3088,7 @@
     </row>
     <row r="4" spans="2:6" ht="25.5">
       <c r="B4" s="104" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="104"/>
       <c r="D4" s="108"/>
@@ -3104,15 +3104,15 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="103" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="103"/>
       <c r="D6" s="107"/>
       <c r="E6" s="107" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="107" t="s">
         <v>74</v>
-      </c>
-      <c r="F6" s="107" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="13.5" thickBot="1">
@@ -3124,7 +3124,7 @@
     </row>
     <row r="8" spans="2:6" ht="39" thickBot="1">
       <c r="B8" s="105" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8" s="106"/>
       <c r="D8" s="109"/>
@@ -3132,7 +3132,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="110" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="2:6">

</xml_diff>

<commit_message>
Working on updating centroid/BOM to work with PCB:NG without errors/changes. Not there yet (four parts to fix)
</commit_message>
<xml_diff>
--- a/board_v12/RGB_Station_v12_BOM_Microchip.xlsx
+++ b/board_v12/RGB_Station_v12_BOM_Microchip.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\RGB_Station\board_v12\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51871DCA-37A4-495C-85D0-6B56C8B50431}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -313,9 +314,6 @@
     <t>U2</t>
   </si>
   <si>
-    <t>74LVC2T45DC,125</t>
-  </si>
-  <si>
     <t>U6</t>
   </si>
   <si>
@@ -467,6 +465,9 @@
   </si>
   <si>
     <t>SW1, SW2</t>
+  </si>
+  <si>
+    <t>150060BS75000</t>
   </si>
 </sst>
 </file>
@@ -1692,7 +1693,7 @@
   <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1700,7 +1701,7 @@
     <col min="1" max="1" width="12.28515625" style="3" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="3" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" style="9" customWidth="1"/>
     <col min="5" max="5" width="37.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="31.28515625" style="3" customWidth="1"/>
@@ -1731,7 +1732,7 @@
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="76" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1991,7 +1992,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="88" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E14" s="90" t="s">
         <v>44</v>
@@ -2039,13 +2040,13 @@
         <v>77</v>
       </c>
       <c r="G15" s="120" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H15" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I15" s="111" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J15" s="53" t="s">
         <v>37</v>
@@ -2072,19 +2073,19 @@
         <v>56</v>
       </c>
       <c r="E16" s="119" t="s">
+        <v>127</v>
+      </c>
+      <c r="F16" s="112" t="s">
         <v>128</v>
       </c>
-      <c r="F16" s="112" t="s">
+      <c r="G16" s="121" t="s">
         <v>129</v>
-      </c>
-      <c r="G16" s="121" t="s">
-        <v>130</v>
       </c>
       <c r="H16" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I16" s="111" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J16" s="53" t="s">
         <v>37</v>
@@ -2108,7 +2109,7 @@
         <v>2</v>
       </c>
       <c r="D17" s="88" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E17" s="119" t="s">
         <v>67</v>
@@ -2147,22 +2148,22 @@
         <v>7</v>
       </c>
       <c r="D18" s="88" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E18" s="111" t="s">
         <v>78</v>
       </c>
       <c r="F18" s="100" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G18" s="124" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H18" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I18" s="111" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J18" s="53" t="s">
         <v>37</v>
@@ -2192,16 +2193,16 @@
         <v>89</v>
       </c>
       <c r="F19" s="100" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G19" s="124" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H19" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I19" s="124" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J19" s="53" t="s">
         <v>37</v>
@@ -2264,22 +2265,22 @@
         <v>3</v>
       </c>
       <c r="D21" s="88" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E21" s="119" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F21" s="100" t="s">
         <v>81</v>
       </c>
       <c r="G21" s="120" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H21" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I21" s="111" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J21" s="53" t="s">
         <v>37</v>
@@ -2351,13 +2352,13 @@
         <v>48</v>
       </c>
       <c r="G23" s="120" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H23" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I23" s="111" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J23" s="53" t="s">
         <v>37</v>
@@ -2390,7 +2391,7 @@
         <v>88</v>
       </c>
       <c r="G24" s="102" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="H24" s="92" t="s">
         <v>33</v>
@@ -2421,7 +2422,7 @@
       </c>
       <c r="D25" s="118"/>
       <c r="E25" s="90" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F25" s="100" t="s">
         <v>58</v>
@@ -2458,19 +2459,19 @@
         <v>95</v>
       </c>
       <c r="E26" s="99" t="s">
+        <v>144</v>
+      </c>
+      <c r="F26" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="F26" s="112" t="s">
-        <v>146</v>
-      </c>
-      <c r="G26" s="122" t="s">
-        <v>96</v>
+      <c r="G26" s="102" t="s">
+        <v>143</v>
       </c>
       <c r="H26" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I26" s="102" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J26" s="53" t="s">
         <v>37</v>
@@ -2491,22 +2492,22 @@
         <v>1</v>
       </c>
       <c r="D27" s="88" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E27" s="119" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F27" s="112" t="s">
         <v>48</v>
       </c>
       <c r="G27" s="122" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H27" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I27" s="111" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J27" s="53" t="s">
         <v>37</v>
@@ -2527,22 +2528,22 @@
         <v>1</v>
       </c>
       <c r="D28" s="88" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" s="111" t="s">
         <v>101</v>
-      </c>
-      <c r="E28" s="111" t="s">
-        <v>102</v>
       </c>
       <c r="F28" s="112" t="s">
         <v>48</v>
       </c>
       <c r="G28" s="124" t="s">
+        <v>130</v>
+      </c>
+      <c r="H28" s="92" t="s">
+        <v>117</v>
+      </c>
+      <c r="I28" s="111" t="s">
         <v>131</v>
-      </c>
-      <c r="H28" s="92" t="s">
-        <v>118</v>
-      </c>
-      <c r="I28" s="111" t="s">
-        <v>132</v>
       </c>
       <c r="J28" s="53" t="s">
         <v>37</v>
@@ -2563,22 +2564,22 @@
         <v>1</v>
       </c>
       <c r="D29" s="88" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E29" s="111" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F29" s="112" t="s">
         <v>51</v>
       </c>
       <c r="G29" s="114" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H29" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I29" s="111" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J29" s="53" t="s">
         <v>37</v>
@@ -2599,22 +2600,22 @@
         <v>2</v>
       </c>
       <c r="D30" s="88" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E30" s="99" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F30" s="100" t="s">
         <v>81</v>
       </c>
       <c r="G30" s="102" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H30" s="92" t="s">
         <v>33</v>
       </c>
       <c r="I30" s="99" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J30" s="53" t="s">
         <v>37</v>
@@ -2694,13 +2695,13 @@
         <v>0</v>
       </c>
       <c r="D34" s="88" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E34" s="111" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F34" s="112" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G34" s="114">
         <v>1984617</v>
@@ -2709,7 +2710,7 @@
         <v>33</v>
       </c>
       <c r="I34" s="111" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J34" s="53" t="s">
         <v>37</v>
@@ -2730,13 +2731,13 @@
         <v>0</v>
       </c>
       <c r="D35" s="88" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E35" s="111" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F35" s="112" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G35" s="114">
         <v>1984633</v>
@@ -2745,7 +2746,7 @@
         <v>33</v>
       </c>
       <c r="I35" s="111" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J35" s="53" t="s">
         <v>37</v>

</xml_diff>